<commit_message>
Modify Document Table Template
</commit_message>
<xml_diff>
--- a/Templates/Document Table.xlsx
+++ b/Templates/Document Table.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BaiduSyncdisk\Projects\COMIGHT\bin\Debug\net8.0-windows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\COMIGHT\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DA3715-96F6-41BB-8231-D683853E52CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC46448F-960E-4C3A-8729-33B277ACC800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="2145" windowWidth="17010" windowHeight="12285" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="小标题" sheetId="8" r:id="rId1"/>
-    <sheet name="大标题首尾" sheetId="1" r:id="rId2"/>
-    <sheet name="主体" sheetId="4" r:id="rId3"/>
+    <sheet name="Headings" sheetId="8" r:id="rId1"/>
+    <sheet name="Title" sheetId="1" r:id="rId2"/>
+    <sheet name="Body" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">主体!$B$2:$C$2270</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Body!$B$2:$C$2270</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>落款</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,14 +57,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>首段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>尾段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>项目</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -105,14 +97,6 @@
   </si>
   <si>
     <t>文首大标题（如：XXX局20XX年工作总结）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文章开头段落（如：20XX年，我局…，现将有关工作开展情况总结如下：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文章结尾段落（如：下阶段，我局将继续…）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -602,31 +586,31 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="12"/>
@@ -634,11 +618,11 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="12"/>
@@ -646,11 +630,11 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="12"/>
@@ -660,7 +644,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="12"/>
@@ -719,10 +703,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -734,70 +718,48 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>18</v>
+      <c r="C3" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5">
-        <v>5</v>
-      </c>
-      <c r="C6" s="8" t="str">
+      <c r="C4" s="8" t="str">
         <f ca="1">TEXT(TODAY(),"yyyy年m月d日")</f>
-        <v>2024年1月27日</v>
+        <v>2024年10月10日</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +777,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C27" sqref="C27"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -833,25 +795,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="12"/>
@@ -859,11 +821,11 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="12"/>
@@ -873,7 +835,7 @@
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="12"/>
@@ -881,11 +843,11 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="12"/>
@@ -893,11 +855,11 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="12"/>
@@ -907,7 +869,7 @@
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="12"/>
@@ -917,7 +879,7 @@
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="12"/>

</xml_diff>

<commit_message>
Update some comments, update Document Table template
</commit_message>
<xml_diff>
--- a/Templates/Document Table.xlsx
+++ b/Templates/Document Table.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\COMIGHT\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC46448F-960E-4C3A-8729-33B277ACC800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F708564-72C5-4DDD-BE7E-80A36E079ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Headings" sheetId="8" r:id="rId1"/>
-    <sheet name="Title" sheetId="1" r:id="rId2"/>
-    <sheet name="Body" sheetId="4" r:id="rId3"/>
+    <sheet name="Title" sheetId="1" r:id="rId1"/>
+    <sheet name="Body" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Body!$B$2:$C$2270</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Body!$B$2:$C$2270</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -39,91 +38,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
-  <si>
-    <t>落款</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标题级别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标题编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>项目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标题级别</t>
-  </si>
-  <si>
-    <t>标题编号</t>
-  </si>
-  <si>
-    <t>完成时限</t>
-  </si>
-  <si>
-    <t>1级</t>
-  </si>
-  <si>
-    <t>2级</t>
-  </si>
-  <si>
-    <t>一级标题文字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>二级标题文字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>（依此类推…）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>正文段落</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文首大标题（如：XXX局20XX年工作总结）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>单位或部门名称（如：XXX局）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>责任部门（人）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分类</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大标题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3级</t>
-  </si>
-  <si>
-    <t>三级标题文字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文字</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+  <si>
+    <t>Headling Level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heading Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lv1</t>
+  </si>
+  <si>
+    <t>Lv2</t>
+  </si>
+  <si>
+    <t>Heading Lv1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heading Lv2</t>
+  </si>
+  <si>
+    <t>Body Text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(etc. …)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Signature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -134,7 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +164,23 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -244,7 +239,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -272,17 +267,20 @@
     <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -568,198 +566,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CEBC8F2-8F45-4A76-906D-B5645268512E}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.75" customWidth="1"/>
-    <col min="3" max="3" width="80.75" customWidth="1"/>
-    <col min="4" max="6" width="12.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A10" xr:uid="{3A2DF922-080C-4AA5-87BC-E7EC6C4DB930}">
-      <formula1>"0级,1级,2级,3级,4级,条,是,接上段"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.75" customWidth="1"/>
-    <col min="3" max="3" width="80.75" customWidth="1"/>
-    <col min="4" max="4" width="12.75" customWidth="1"/>
+    <col min="1" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="80.77734375" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="str">
-        <f ca="1">TEXT(TODAY(),"yyyy年m月d日")</f>
-        <v>2024年10月10日</v>
+      <c r="C4" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -769,7 +633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F10"/>
@@ -777,135 +641,138 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C27" sqref="C27"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A10"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.75" customWidth="1"/>
-    <col min="3" max="3" width="80.75" customWidth="1"/>
-    <col min="4" max="6" width="12.75" customWidth="1"/>
+    <col min="1" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="80.77734375" customWidth="1"/>
+    <col min="4" max="6" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="11" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>8</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="11" t="s">
-        <v>14</v>
-      </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A10" xr:uid="{6DB1F0B4-511A-47F8-A4DC-22FA02B7A236}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A8:A10" xr:uid="{6DB1F0B4-511A-47F8-A4DC-22FA02B7A236}">
       <formula1>"0级,1级,2级,3级,4级,条,是,接上段"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A7" xr:uid="{2BD6AE84-732F-4EDB-B78F-F2EEFF92BFE2}">
+      <formula1>"Lv0,Lv1,Lv2,Lv3,Lv4,Enum.,Itm.,Immed."</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>